<commit_message>
introduced pearson's correlation coefficient
</commit_message>
<xml_diff>
--- a/Metric comparison.xlsx
+++ b/Metric comparison.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preston/SCH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDD1668-8D0D-7949-8E0D-83BD3B159301}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A810CD2-E8B0-9E40-A354-684B12D4CD1A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Sheet 1'!$C$16:$C$42</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Sheet 1'!$F$15</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Sheet 1'!$F$16:$F$42</definedName>
+  </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -137,14 +142,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,7 +549,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -557,7 +562,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>JR</a:t>
                 </a:r>
               </a:p>
@@ -576,7 +581,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -661,7 +666,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -674,7 +679,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>MR</a:t>
                 </a:r>
               </a:p>
@@ -693,7 +698,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -836,7 +841,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1400"/>
               <a:t>JR vs. UR</a:t>
             </a:r>
           </a:p>
@@ -1183,7 +1188,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1196,7 +1201,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>JR</a:t>
                 </a:r>
               </a:p>
@@ -1215,7 +1220,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1300,7 +1305,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1313,7 +1318,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>UR</a:t>
                 </a:r>
               </a:p>
@@ -1332,7 +1337,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1527,6 +1532,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Sheet 1'!$C$16:$C$42</c:f>
@@ -1753,7 +1802,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1766,7 +1815,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>JR</a:t>
                 </a:r>
               </a:p>
@@ -1785,7 +1834,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1870,7 +1919,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1883,7 +1932,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>AR</a:t>
                 </a:r>
               </a:p>
@@ -1902,7 +1951,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4094,33 +4143,33 @@
   </sheetPr>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="115" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
@@ -4569,7 +4618,7 @@
       <c r="M13" s="5">
         <v>0.47742480926855241</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="N13" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4591,7 +4640,7 @@
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="2">
@@ -4611,7 +4660,7 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="7"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="2">
         <v>0.53858599925443951</v>
       </c>
@@ -4629,7 +4678,7 @@
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="2">
         <v>0.47050850829319807</v>
       </c>
@@ -4647,7 +4696,7 @@
       <c r="A19" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="2">
         <v>0.50496979105771123</v>
       </c>
@@ -4665,7 +4714,7 @@
       <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="7"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="2">
         <v>0.5096188532838325</v>
       </c>
@@ -4683,7 +4732,7 @@
       <c r="A21" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="7"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2">
         <v>0.5969735049853524</v>
       </c>
@@ -4701,7 +4750,7 @@
       <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="2">
         <v>0.56208632441205808</v>
       </c>
@@ -4719,7 +4768,7 @@
       <c r="A23" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="2">
         <v>0.63728648338812521</v>
       </c>
@@ -4737,7 +4786,7 @@
       <c r="A24" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="7"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="2">
         <v>0.56773366258912705</v>
       </c>
@@ -4755,7 +4804,7 @@
       <c r="A25" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="2">
@@ -4775,7 +4824,7 @@
       <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="7"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="2">
         <v>0.51005247161515188</v>
       </c>
@@ -4793,7 +4842,7 @@
       <c r="A27" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="7"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="2">
         <v>0.47965439637880886</v>
       </c>
@@ -4811,7 +4860,7 @@
       <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="2">
         <v>0.51500438470925736</v>
       </c>
@@ -4829,7 +4878,7 @@
       <c r="A29" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="7"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="2">
         <v>0.53641693764173493</v>
       </c>
@@ -4847,7 +4896,7 @@
       <c r="A30" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="2">
         <v>0.41913344266680425</v>
       </c>
@@ -4865,7 +4914,7 @@
       <c r="A31" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="2">
         <v>0.49665467778295708</v>
       </c>
@@ -4883,7 +4932,7 @@
       <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="2">
         <v>0.455640108420101</v>
       </c>
@@ -4901,7 +4950,7 @@
       <c r="A33" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="2">
         <v>0.33819828007046304</v>
       </c>
@@ -4919,7 +4968,7 @@
       <c r="A34" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="2">
@@ -4939,7 +4988,7 @@
       <c r="A35" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="7"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="2">
         <v>0.54731214792249128</v>
       </c>
@@ -4957,7 +5006,7 @@
       <c r="A36" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="7"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="2">
         <v>0.45598557515242999</v>
       </c>
@@ -4975,7 +5024,7 @@
       <c r="A37" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="7"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="2">
         <v>0.50122463687124896</v>
       </c>
@@ -4993,7 +5042,7 @@
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="2">
         <v>0.53590927077581019</v>
       </c>
@@ -5011,7 +5060,7 @@
       <c r="A39" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="7"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="2">
         <v>0.61505659339300711</v>
       </c>
@@ -5029,7 +5078,7 @@
       <c r="A40" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="7"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="2">
         <v>0.56601379158678178</v>
       </c>
@@ -5047,7 +5096,7 @@
       <c r="A41" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="7"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="2">
         <v>0.64494397406886905</v>
       </c>
@@ -5065,7 +5114,7 @@
       <c r="A42" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="7"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="2">
         <v>0.62679037446231911</v>
       </c>
@@ -5081,13 +5130,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B25:B33"/>
+    <mergeCell ref="B34:B42"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="B16:B24"/>
-    <mergeCell ref="B25:B33"/>
-    <mergeCell ref="B34:B42"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>